<commit_message>
Fix: Get Transaction Data works, and all lists is sorted by descending order.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -158,9 +158,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>SheetNames</t>
+  </si>
+  <si>
+    <t>Handläggarkö</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -624,7 +624,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -655,10 +655,10 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1732,13 +1732,13 @@
     </row>
     <row r="4" spans="1:26" ht="36" customHeight="1">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2838,7 +2838,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2887,37 +2887,37 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Updated sum and compare excel and procapita.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -189,6 +189,30 @@
   </si>
   <si>
     <t>Handläggarkö</t>
+  </si>
+  <si>
+    <t>ColumnsInAktualiseringar</t>
+  </si>
+  <si>
+    <t>KolumnerIAktualiseringar</t>
+  </si>
+  <si>
+    <t>ColumnsInBevakningar</t>
+  </si>
+  <si>
+    <t>ColumnsInMedicalRecords</t>
+  </si>
+  <si>
+    <t>ColumnsInUtredningar</t>
+  </si>
+  <si>
+    <t>KolumnerIBevakningar</t>
+  </si>
+  <si>
+    <t>KolumnerIMedicalRecords</t>
+  </si>
+  <si>
+    <t>KolumnerIUtredningar</t>
   </si>
 </sst>
 </file>
@@ -2838,7 +2862,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2920,10 +2944,38 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Updating dashboard. Started Send mail
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="9750" windowHeight="9795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -213,6 +213,24 @@
   </si>
   <si>
     <t>KolumnerIUtredningar</t>
+  </si>
+  <si>
+    <t>MailBodyText</t>
+  </si>
+  <si>
+    <t>MailSenderAddress</t>
+  </si>
+  <si>
+    <t>MailSenderName</t>
+  </si>
+  <si>
+    <t>MailServerAddress</t>
+  </si>
+  <si>
+    <t>MailServerPort</t>
+  </si>
+  <si>
+    <t>MailSubject</t>
   </si>
 </sst>
 </file>
@@ -2859,10 +2877,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2976,12 +2994,54 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -3966,7 +4026,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: Sending mail and copying files before uppdating them.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>MailSubject</t>
+  </si>
+  <si>
+    <t>TempFolderFilePath</t>
   </si>
 </sst>
 </file>
@@ -2880,7 +2883,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3042,7 +3045,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: new columns in dt_settings. new sort for bevakningar.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -209,9 +209,6 @@
     <t>KolumnerIUtredningar</t>
   </si>
   <si>
-    <t>MailBodyText</t>
-  </si>
-  <si>
     <t>MailSenderAddress</t>
   </si>
   <si>
@@ -255,6 +252,27 @@
   </si>
   <si>
     <t>NrOfDaysToSearchInUtredning</t>
+  </si>
+  <si>
+    <t>MailBodyTextFirstPart</t>
+  </si>
+  <si>
+    <t>MailBodyTextJournalanteckningar</t>
+  </si>
+  <si>
+    <t>MailBodyTextBevakningar</t>
+  </si>
+  <si>
+    <t>MailBodyTextLastPart</t>
+  </si>
+  <si>
+    <t>MailBodyTextMedicalRecords</t>
+  </si>
+  <si>
+    <t>MailBodyTextUtredningar</t>
+  </si>
+  <si>
+    <t>MailBodyTextAktualiseringar</t>
   </si>
 </sst>
 </file>
@@ -720,7 +738,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
@@ -1822,7 +1840,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1924,7 +1942,7 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>40</v>
@@ -2915,14 +2933,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
@@ -3079,27 +3097,27 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" t="s">
-        <v>67</v>
+      <c r="A16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
@@ -3107,14 +3125,49 @@
         <v>76</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Libupdated. Filepath to application needed.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>MailBodyTextAktualiseringar</t>
+  </si>
+  <si>
+    <t>ApplicationFilePath</t>
   </si>
 </sst>
 </file>
@@ -2934,7 +2937,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3168,7 +3171,14 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: New days for bevakning.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>FolderName</t>
+  </si>
+  <si>
+    <t>DagarFramåtBevakning</t>
   </si>
 </sst>
 </file>
@@ -2942,7 +2945,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3192,7 +3195,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Try catch around kill, checks if wants email.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>DagarFramåtBevakning</t>
+  </si>
+  <si>
+    <t>DagarFramåtJournalanteckningar</t>
+  </si>
+  <si>
+    <t>DagarFramåtUtredning</t>
   </si>
 </sst>
 </file>
@@ -2945,7 +2951,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3203,8 +3209,22 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Copy old working file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -288,6 +288,15 @@
   </si>
   <si>
     <t>DagarFramåtUtredning</t>
+  </si>
+  <si>
+    <t>CoruptFileTextToExcel</t>
+  </si>
+  <si>
+    <t>CoruptFileTextToEmail</t>
+  </si>
+  <si>
+    <t>MailSubjectCoruptFile</t>
   </si>
 </sst>
 </file>
@@ -2951,7 +2960,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3225,9 +3234,30 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix:  new way to update to excel, new way to generate add/remove list.
Added retry for open excel in manipulateDtFromExcel, changed logs.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>MailSubjectCoruptFile</t>
+  </si>
+  <si>
+    <t>DaysToShowBev</t>
   </si>
 </sst>
 </file>
@@ -2960,7 +2963,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3258,22 +3261,29 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>